<commit_message>
Added results of eval002
</commit_message>
<xml_diff>
--- a/Evaluation/ML_Results/ml_results.xlsx
+++ b/Evaluation/ML_Results/ml_results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,19 +409,24 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>roc_auc_overall_validation</t>
+          <t>roc_auc_overall_validation_x</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>roc_auc_overall_validation_y</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1:26PM CET on Nov 24, 2022</t>
+          <t xml:space="preserve"> 1:59PM CET on Nov 24, 2022</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eval001</t>
+          <t>eval002</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -431,24 +436,25 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GradientBoostingClassifier</t>
+          <t>RandomForestClassifier</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.9801980198019802</v>
+        <v>0.8514851485148515</v>
       </c>
       <c r="F2" t="n">
-        <v>0.872904761904762</v>
+        <v>0.9210238095238095</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>/data/favel/Evaluation/eval001</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
+          <t>/data/favel/Evaluation/eval002</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added results of eval001 and eval002
</commit_message>
<xml_diff>
--- a/Evaluation/ML_Results/ml_results.xlsx
+++ b/Evaluation/ML_Results/ml_results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,53 +409,86 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>roc_auc_overall_validation_x</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>roc_auc_overall_validation_y</t>
+          <t>roc_auc_overall_validation</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1:59PM CET on Nov 24, 2022</t>
+          <t>11:19AM CET on Nov 30, 2022</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>eval001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>/home/sascha/Projects/BPDP-Dataset_2022/BPDP_Dataset/</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>GradientBoostingClassifier</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9801980198019802</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>/home/sascha/Projects/favel/Evaluation/eval001</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.6747572815533981</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>11:19AM CET on Nov 30, 2022</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>eval002</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>/data/dataset/BPDP-Dataset_2022/BPDP_Dataset/</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>/home/sascha/Projects/BPDP-Dataset_2022/BPDP_Dataset/</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>RandomForestClassifier</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>0.8514851485148515</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.9210238095238095</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>/data/favel/Evaluation/eval002</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>0.5</v>
+      <c r="E3" t="n">
+        <v>0.8811881188118812</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9268571428571428</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>/home/sascha/Projects/favel/Evaluation/eval002</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.6699029126213593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run a local experiment with Gradient boosting on BPDP
</commit_message>
<xml_diff>
--- a/Evaluation/ML_Results/ml_results.xlsx
+++ b/Evaluation/ML_Results/ml_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -66,6 +65,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +558,45 @@
         <v>0.6699029126213593</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3:02PM CET on Nov 30, 2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>eval003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>./../Datasets/BPDP-Dataset_2022/BPDP_Dataset/</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>GradientBoostingClassifier</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9801980198019802</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8480000000000001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>/media/ltphen/Ulife/project/school/pg/github/favel/Evaluation/eval003</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.5922330097087378</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>